<commit_message>
✅ Agrega 'Disponible' en fechas clave para pruebas de disponibilidad
</commit_message>
<xml_diff>
--- a/Reservas_Alma_Glamping.xlsx
+++ b/Reservas_Alma_Glamping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cavuf\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766D58E5-D103-4284-A547-AEA1DAAF5809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60663CB1-6FC7-4198-8DE2-7D75AA460387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3552" yWindow="3360" windowWidth="16224" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reservas" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="7">
   <si>
     <t>Fecha</t>
   </si>
@@ -39,13 +39,16 @@
   <si>
     <t>reservado</t>
   </si>
+  <si>
+    <t>Disponible</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -383,13 +386,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="16" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.44140625" customWidth="1"/>
     <col min="3" max="3" width="18.21875" customWidth="1"/>
     <col min="4" max="4" width="20.5546875" customWidth="1"/>
@@ -397,7 +400,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -478,21 +481,69 @@
       <c r="A7" s="1">
         <v>45803</v>
       </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45804</v>
       </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45805</v>
       </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>45806</v>
       </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -549,26 +600,86 @@
       <c r="A14" s="1">
         <v>45810</v>
       </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>45811</v>
       </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>45812</v>
       </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>45813</v>
       </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>45814</v>
       </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -608,26 +719,86 @@
       <c r="A21" s="1">
         <v>45817</v>
       </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45818</v>
       </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45819</v>
       </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>45820</v>
       </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45821</v>
       </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
@@ -667,26 +838,86 @@
       <c r="A28" s="1">
         <v>45824</v>
       </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>45825</v>
       </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>45826</v>
       </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>45827</v>
       </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>45828</v>
       </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
@@ -726,478 +957,1619 @@
       <c r="A35" s="1">
         <v>45831</v>
       </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>45832</v>
       </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>45833</v>
       </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>45834</v>
       </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>45835</v>
       </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>45836</v>
       </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>45837</v>
       </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>45838</v>
       </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>45839</v>
       </c>
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>45840</v>
       </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>45841</v>
       </c>
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45842</v>
       </c>
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45843</v>
       </c>
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>45844</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>45845</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>45846</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>45847</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>45848</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>45849</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>45850</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>45851</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>45852</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>45853</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>45854</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>45855</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>45856</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>45857</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>45858</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>45859</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>45860</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>45861</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>45862</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>45863</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>45864</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>45865</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>45866</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>6</v>
+      </c>
+      <c r="C70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>45867</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>45868</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>45869</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>45870</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>6</v>
+      </c>
+      <c r="C74" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>45871</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>45872</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>45873</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>45874</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>45875</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>45876</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>45877</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>45878</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>45879</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" t="s">
+        <v>6</v>
+      </c>
+      <c r="E83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>45880</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>45881</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>45882</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>45883</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>45884</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>6</v>
+      </c>
+      <c r="C88" t="s">
+        <v>6</v>
+      </c>
+      <c r="D88" t="s">
+        <v>6</v>
+      </c>
+      <c r="E88" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>45885</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" t="s">
+        <v>6</v>
+      </c>
+      <c r="E89" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>45886</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" t="s">
+        <v>6</v>
+      </c>
+      <c r="E90" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>45887</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>6</v>
+      </c>
+      <c r="C91" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>45888</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92" t="s">
+        <v>6</v>
+      </c>
+      <c r="C92" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" t="s">
+        <v>6</v>
+      </c>
+      <c r="E92" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>45889</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>45890</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94" t="s">
+        <v>6</v>
+      </c>
+      <c r="D94" t="s">
+        <v>6</v>
+      </c>
+      <c r="E94" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>45891</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>6</v>
+      </c>
+      <c r="C95" t="s">
+        <v>6</v>
+      </c>
+      <c r="D95" t="s">
+        <v>6</v>
+      </c>
+      <c r="E95" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>45892</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" t="s">
+        <v>6</v>
+      </c>
+      <c r="E96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>45893</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" t="s">
+        <v>6</v>
+      </c>
+      <c r="E97" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>45894</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>6</v>
+      </c>
+      <c r="C98" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" t="s">
+        <v>6</v>
+      </c>
+      <c r="E98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>45895</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>6</v>
+      </c>
+      <c r="C99" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" t="s">
+        <v>6</v>
+      </c>
+      <c r="E99" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>45896</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>6</v>
+      </c>
+      <c r="C100" t="s">
+        <v>6</v>
+      </c>
+      <c r="D100" t="s">
+        <v>6</v>
+      </c>
+      <c r="E100" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>45897</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>6</v>
+      </c>
+      <c r="C101" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" t="s">
+        <v>6</v>
+      </c>
+      <c r="E101" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>45898</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>6</v>
+      </c>
+      <c r="C102" t="s">
+        <v>6</v>
+      </c>
+      <c r="D102" t="s">
+        <v>6</v>
+      </c>
+      <c r="E102" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>45899</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>6</v>
+      </c>
+      <c r="C103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D103" t="s">
+        <v>6</v>
+      </c>
+      <c r="E103" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>45900</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>6</v>
+      </c>
+      <c r="C104" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" t="s">
+        <v>6</v>
+      </c>
+      <c r="E104" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>45901</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>6</v>
+      </c>
+      <c r="C105" t="s">
+        <v>6</v>
+      </c>
+      <c r="D105" t="s">
+        <v>6</v>
+      </c>
+      <c r="E105" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>45902</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>6</v>
+      </c>
+      <c r="C106" t="s">
+        <v>6</v>
+      </c>
+      <c r="D106" t="s">
+        <v>6</v>
+      </c>
+      <c r="E106" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>45903</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>6</v>
+      </c>
+      <c r="C107" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" t="s">
+        <v>6</v>
+      </c>
+      <c r="E107" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>45904</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
+        <v>6</v>
+      </c>
+      <c r="C108" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108" t="s">
+        <v>6</v>
+      </c>
+      <c r="E108" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>45905</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>45906</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
+        <v>6</v>
+      </c>
+      <c r="C110" t="s">
+        <v>6</v>
+      </c>
+      <c r="D110" t="s">
+        <v>6</v>
+      </c>
+      <c r="E110" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>45907</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>6</v>
+      </c>
+      <c r="C111" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" t="s">
+        <v>6</v>
+      </c>
+      <c r="E111" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>45908</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
+        <v>6</v>
+      </c>
+      <c r="C112" t="s">
+        <v>6</v>
+      </c>
+      <c r="D112" t="s">
+        <v>6</v>
+      </c>
+      <c r="E112" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>45909</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>6</v>
+      </c>
+      <c r="C113" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" t="s">
+        <v>6</v>
+      </c>
+      <c r="E113" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>45910</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
+        <v>6</v>
+      </c>
+      <c r="C114" t="s">
+        <v>6</v>
+      </c>
+      <c r="D114" t="s">
+        <v>6</v>
+      </c>
+      <c r="E114" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>45911</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
+        <v>6</v>
+      </c>
+      <c r="C115" t="s">
+        <v>6</v>
+      </c>
+      <c r="D115" t="s">
+        <v>6</v>
+      </c>
+      <c r="E115" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>45912</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B116" t="s">
+        <v>6</v>
+      </c>
+      <c r="C116" t="s">
+        <v>6</v>
+      </c>
+      <c r="D116" t="s">
+        <v>6</v>
+      </c>
+      <c r="E116" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>45913</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
+        <v>6</v>
+      </c>
+      <c r="C117" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" t="s">
+        <v>6</v>
+      </c>
+      <c r="E117" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>45914</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>6</v>
+      </c>
+      <c r="C118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D118" t="s">
+        <v>6</v>
+      </c>
+      <c r="E118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>45915</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
+        <v>6</v>
+      </c>
+      <c r="C119" t="s">
+        <v>6</v>
+      </c>
+      <c r="D119" t="s">
+        <v>6</v>
+      </c>
+      <c r="E119" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>45916</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>6</v>
+      </c>
+      <c r="C120" t="s">
+        <v>6</v>
+      </c>
+      <c r="D120" t="s">
+        <v>6</v>
+      </c>
+      <c r="E120" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>45917</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>6</v>
+      </c>
+      <c r="C121" t="s">
+        <v>6</v>
+      </c>
+      <c r="D121" t="s">
+        <v>6</v>
+      </c>
+      <c r="E121" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>45918</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
+        <v>6</v>
+      </c>
+      <c r="C122" t="s">
+        <v>6</v>
+      </c>
+      <c r="D122" t="s">
+        <v>6</v>
+      </c>
+      <c r="E122" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>45919</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B123" t="s">
+        <v>6</v>
+      </c>
+      <c r="C123" t="s">
+        <v>6</v>
+      </c>
+      <c r="D123" t="s">
+        <v>6</v>
+      </c>
+      <c r="E123" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>45920</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
+        <v>6</v>
+      </c>
+      <c r="C124" t="s">
+        <v>6</v>
+      </c>
+      <c r="D124" t="s">
+        <v>6</v>
+      </c>
+      <c r="E124" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>45921</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
+        <v>6</v>
+      </c>
+      <c r="C125" t="s">
+        <v>6</v>
+      </c>
+      <c r="D125" t="s">
+        <v>6</v>
+      </c>
+      <c r="E125" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>45922</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>6</v>
+      </c>
+      <c r="C126" t="s">
+        <v>6</v>
+      </c>
+      <c r="D126" t="s">
+        <v>6</v>
+      </c>
+      <c r="E126" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>45923</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
+        <v>6</v>
+      </c>
+      <c r="C127" t="s">
+        <v>6</v>
+      </c>
+      <c r="D127" t="s">
+        <v>6</v>
+      </c>
+      <c r="E127" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>45924</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B128" t="s">
+        <v>6</v>
+      </c>
+      <c r="C128" t="s">
+        <v>6</v>
+      </c>
+      <c r="D128" t="s">
+        <v>6</v>
+      </c>
+      <c r="E128" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>45925</v>
       </c>
+      <c r="B129" t="s">
+        <v>6</v>
+      </c>
+      <c r="C129" t="s">
+        <v>6</v>
+      </c>
+      <c r="D129" t="s">
+        <v>6</v>
+      </c>
+      <c r="E129" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📅 Forzado: actualización de archivo Excel con fechas disponibles
</commit_message>
<xml_diff>
--- a/Reservas_Alma_Glamping.xlsx
+++ b/Reservas_Alma_Glamping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cavuf\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60663CB1-6FC7-4198-8DE2-7D75AA460387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D4A3F8-A360-4A86-A0AF-A930FC85195C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3552" yWindow="3360" windowWidth="16224" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="8">
   <si>
     <t>Fecha</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Disponible</t>
+  </si>
+  <si>
+    <t>Reservado</t>
   </si>
 </sst>
 </file>
@@ -386,8 +389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A131" sqref="A131"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1944,13 +1947,13 @@
         <v>45889</v>
       </c>
       <c r="B93" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C93" t="s">
         <v>6</v>
       </c>
       <c r="D93" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E93" t="s">
         <v>6</v>
@@ -2474,10 +2477,10 @@
         <v>6</v>
       </c>
       <c r="C124" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D124" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E124" t="s">
         <v>6</v>

</xml_diff>